<commit_message>
update excel test file
</commit_message>
<xml_diff>
--- a/src/test/resources/test_excel_table.xlsx
+++ b/src/test/resources/test_excel_table.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richarddiamond/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richarddiamond/Documents/Data/Projects/yariEditor/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A172CF9E-A884-9C49-8683-E343FC8B6EFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF6C77F-77EF-3943-BE1C-304FFAA72E32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22840" yWindow="5660" windowWidth="28040" windowHeight="17440" xr2:uid="{B8B3E2A1-7A73-B145-8B61-21800F31C950}"/>
+    <workbookView xWindow="10520" yWindow="12900" windowWidth="28040" windowHeight="17440" xr2:uid="{B8B3E2A1-7A73-B145-8B61-21800F31C950}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DecisionTable" sheetId="2" r:id="rId1"/>
+    <sheet name="Validation" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Type</t>
   </si>
@@ -57,51 +58,98 @@
     <t>==</t>
   </si>
   <si>
-    <t>testMethod</t>
-  </si>
-  <si>
-    <t>alphaMethod</t>
-  </si>
-  <si>
-    <t>betaMethod</t>
-  </si>
-  <si>
-    <t>actionMethod</t>
-  </si>
-  <si>
-    <t>meowth</t>
-  </si>
-  <si>
-    <t>beedrill</t>
-  </si>
-  <si>
-    <t>pikachu</t>
-  </si>
-  <si>
-    <t>bulbasuar</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>mew</t>
-  </si>
-  <si>
-    <t>nope</t>
-  </si>
-  <si>
-    <t>ahhaha</t>
-  </si>
-  <si>
-    <t>aang</t>
+    <t>!=</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>isValid</t>
+  </si>
+  <si>
+    <t>getSize</t>
+  </si>
+  <si>
+    <t>setNumber</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>jane</t>
+  </si>
+  <si>
+    <t>matthew</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,10 +165,39 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -129,9 +206,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,130 +544,262 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7A8DB6-463C-6248-BE5E-D75E6789865C}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C309088-7BF0-A248-BDF8-8C914C9F9E90}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E6">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="b">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9273B70-A3A8-C245-986E-C0A0DD1D4CE1}">
+          <x14:formula1>
+            <xm:f>Validation!$C$1:$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:Z1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{588A6334-C656-1748-AC11-3B7715C579C6}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:Z2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A53A93AF-995F-3342-9118-B2BFD8944CA8}">
+          <x14:formula1>
+            <xm:f>Validation!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:Z3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7561270-BEE3-2C47-BA9D-B8EF0C8435D4}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Custom exception for excel importing, unit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test_excel_table.xlsx
+++ b/src/test/resources/test_excel_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richarddiamond/Documents/Data/Projects/yariEditor/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richarddiamond/Documents/Development/Projects/yariEditor/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF6C77F-77EF-3943-BE1C-304FFAA72E32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15320CB-DD4E-144E-BB59-4CA1AED6EB8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10520" yWindow="12900" windowWidth="28040" windowHeight="17440" xr2:uid="{B8B3E2A1-7A73-B145-8B61-21800F31C950}"/>
+    <workbookView xWindow="5560" yWindow="3560" windowWidth="28040" windowHeight="16760" xr2:uid="{B8B3E2A1-7A73-B145-8B61-21800F31C950}"/>
   </bookViews>
   <sheets>
     <sheet name="DecisionTable" sheetId="2" r:id="rId1"/>
@@ -548,7 +548,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,16 +560,16 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -577,16 +577,16 @@
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -594,15 +594,16 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>